<commit_message>
Agregar envio de correo con formato html. Wednesday 2025-01-29
</commit_message>
<xml_diff>
--- a/informeEjecutivo/Formato_ordenes.xlsx
+++ b/informeEjecutivo/Formato_ordenes.xlsx
@@ -8,20 +8,20 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="18-01-2025" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Total" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'18-01-2025'!$A$1:$M$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'18-01-2025'!$A$9:$M$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_195E5D94_9DB5_439B_9C35_98BA6A3DE53A_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_195F1ACD_5C9F_4B29_BBFE_2492BB71E3F5_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_2CF9F157_7EE3_4708_A32E_8E85D70E0803_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_3D64FB1A_3A94_421D_AD42_CC4BEB7898BA_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_4DD43DB5_5323_4E35_8897_247879ADDA2F_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_BB6917AA_8273_48F5_9BEB_A0A974EB6292_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_EA197D2E_6639_4F0D_A9B5_6721AE67A1B7_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="Z_FEF3668A_BBEA_4AA2_9DE0_F9CF707A13A1_.wvu.PrintTitles" vbProcedure="false">'18-01-2025'!$8:$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Total!$A$1:$M$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Total!$A$9:$M$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_195E5D94_9DB5_439B_9C35_98BA6A3DE53A_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_195F1ACD_5C9F_4B29_BBFE_2492BB71E3F5_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_2CF9F157_7EE3_4708_A32E_8E85D70E0803_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_3D64FB1A_3A94_421D_AD42_CC4BEB7898BA_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_4DD43DB5_5323_4E35_8897_247879ADDA2F_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_BB6917AA_8273_48F5_9BEB_A0A974EB6292_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_EA197D2E_6639_4F0D_A9B5_6721AE67A1B7_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="Z_FEF3668A_BBEA_4AA2_9DE0_F9CF707A13A1_.wvu.PrintTitles" vbProcedure="false">Total!$8:$9</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -419,9 +419,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1888560</xdr:colOff>
+      <xdr:colOff>1888200</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -435,7 +435,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="460800" y="76320"/>
-          <a:ext cx="2045520" cy="951480"/>
+          <a:ext cx="2045160" cy="951120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>